<commit_message>
Submit methods in controllers
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjust\Desktop\Universidad\4o\Semestre 2\[DAD] Desarrollo de aplicaciones distribuidas\Práctica\GamePost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F96A5F-133C-40D4-A7F5-C8C1536DFADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0205B47F-373F-43CD-B257-6B8D502ED4A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -289,6 +289,21 @@
   </si>
   <si>
     <t>CustomList</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>new Content(</t>
+  </si>
+  <si>
+    <t>userRepository.save(new User(username, password));</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>INSERT INTO User VALUES(username, password)</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1081,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,8 +1111,12 @@
         <v>25</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1246,8 +1265,8 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,6 +1277,7 @@
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1303,8 +1323,12 @@
         <v>68</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
@@ -1338,7 +1362,10 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="1" t="str">
+        <f>CONCATENATE("userRepository.save(new User(",C3,", ",D3,"));")</f>
+        <v>userRepository.save(new User(Julen, julen));</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
@@ -1372,7 +1399,10 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="1" t="str">
+        <f>CONCATENATE("userRepository.save(new User(",C4,", ",D4,"));")</f>
+        <v>userRepository.save(new User(Mariam, mariam));</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
@@ -1419,8 +1449,12 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
@@ -1436,7 +1470,10 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1" t="str">
+        <f>CONCATENATE("INSERT INTO User VALUES(",C3,", ",D3,")")</f>
+        <v>INSERT INTO User VALUES(Julen, julen)</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
@@ -1452,7 +1489,10 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1" t="str">
+        <f>CONCATENATE("INSERT INTO User VALUES(",C4,", ",D4,")")</f>
+        <v>INSERT INTO User VALUES(Mariam, mariam)</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>

</xml_diff>